<commit_message>
created a function to train and predict based on specified models
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nitanshjain/Documents/Projects/Shopper_Intent_Prediction/shopper-intent-prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25EB610F-2087-D848-B630-8049AC556C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBA15BC0-FD2C-4742-BF5F-08A204850897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{A310C6DF-D540-3C4A-BE5D-7C178FE1B99A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15800" windowHeight="18000" xr2:uid="{A310C6DF-D540-3C4A-BE5D-7C178FE1B99A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MI" sheetId="1" r:id="rId1"/>
+    <sheet name="MRMR" sheetId="2" r:id="rId2"/>
+    <sheet name="MI_MRMR" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,15 +37,50 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>f1_score</t>
+  </si>
+  <si>
+    <t>AUC</t>
+  </si>
+  <si>
+    <t>Accuracy</t>
+  </si>
+  <si>
+    <t>Percentile</t>
+  </si>
+  <si>
+    <t>Sample_id</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFCCCCCC"/>
+      <name val="Menlo"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,8 +103,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -83,6 +121,22 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{46B0541A-2B00-714A-B082-6EAB4BFA6480}" name="Table1" displayName="Table1" ref="A1:G11" totalsRowShown="0">
+  <autoFilter ref="A1:G11" xr:uid="{46B0541A-2B00-714A-B082-6EAB4BFA6480}"/>
+  <tableColumns count="7">
+    <tableColumn id="1" xr3:uid="{440561F7-410D-BA49-BD07-B26C25CB9FA2}" name="Sample_id"/>
+    <tableColumn id="2" xr3:uid="{EA1805AA-2C7B-E14A-830B-992F362E2276}" name="Features"/>
+    <tableColumn id="3" xr3:uid="{6426A6EF-049F-0E4F-AAA7-7B14745EE220}" name="Percentile"/>
+    <tableColumn id="4" xr3:uid="{931B1917-6D4A-734E-AFC4-F159731B2BDB}" name="Model"/>
+    <tableColumn id="5" xr3:uid="{E8548598-476B-C94F-8DCD-C50B18C6C361}" name="f1_score"/>
+    <tableColumn id="6" xr3:uid="{CB1C0C37-19F2-7B43-84FB-425A7C756B93}" name="AUC"/>
+    <tableColumn id="7" xr3:uid="{6E932C9C-B02A-2842-9913-BAC8ACB9563B}" name="Accuracy"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,9 +436,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A07508F-8AEA-7444-8D09-8999E9C7BCFC}">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.75480769230769196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.79807692307692302</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.82692307692307598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FDE0B2-CB56-494E-AECA-CC511896DF33}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7155D06F-2D7A-1C45-B1E1-F5A2A0D7DB6F}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>